<commit_message>
atualizando o simulador com os dados até maio
</commit_message>
<xml_diff>
--- a/Base Simulador.xlsx
+++ b/Base Simulador.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="11">
   <si>
     <t>KPI1</t>
   </si>
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,28 +444,28 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>212527.373419</v>
+        <v>247105.769379</v>
       </c>
       <c r="C2">
-        <v>320858.2901905637</v>
+        <v>352421.8203048419</v>
       </c>
       <c r="D2">
         <v>0.999999995</v>
       </c>
       <c r="E2">
-        <v>24364334.86480342</v>
+        <v>33686531.32457296</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2">
-        <v>88161948.23425201</v>
+        <v>93328618.23009101</v>
       </c>
       <c r="H2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I2">
-        <v>117055004.6561</v>
+        <v>128432757.136888</v>
       </c>
       <c r="J2" t="s">
         <v>9</v>
@@ -476,28 +476,28 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>165675.579971</v>
+        <v>217838.694291</v>
       </c>
       <c r="C3">
-        <v>277665.8280495264</v>
+        <v>335995.3795279213</v>
       </c>
       <c r="D3">
         <v>0.999999995</v>
       </c>
       <c r="E3">
-        <v>-1928444.340090676</v>
+        <v>-4332350.325584246</v>
       </c>
       <c r="F3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G3">
-        <v>106378958.82258</v>
+        <v>103079563.372284</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I3">
-        <v>89673511.2256173</v>
+        <v>88394348.4730044</v>
       </c>
       <c r="J3" t="s">
         <v>9</v>
@@ -508,28 +508,28 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>153320.9036899999</v>
+        <v>266863.3809499999</v>
       </c>
       <c r="C4">
-        <v>244088.773104699</v>
+        <v>295364.757463744</v>
       </c>
       <c r="D4">
-        <v>-1.000000006</v>
+        <v>-7E-09</v>
       </c>
       <c r="E4">
-        <v>5562878.910695469</v>
+        <v>6872304.585514694</v>
       </c>
       <c r="F4">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G4">
-        <v>58067874.7513764</v>
+        <v>60776319.5446833</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I4">
-        <v>50607518.8179473</v>
+        <v>53121362.2945006</v>
       </c>
       <c r="J4" t="s">
         <v>9</v>
@@ -540,28 +540,28 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>63667.406661</v>
+        <v>84468.887581</v>
       </c>
       <c r="C5">
-        <v>188773.3472441281</v>
+        <v>228429.1621248172</v>
       </c>
       <c r="D5">
-        <v>4.999999986</v>
+        <v>5.999999985</v>
       </c>
       <c r="E5">
-        <v>10337481.2447754</v>
+        <v>13833365.16757777</v>
       </c>
       <c r="F5">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G5">
-        <v>74881267.7972614</v>
+        <v>81070536.6320347</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I5">
-        <v>60429692.9273029</v>
+        <v>65436270.2644522</v>
       </c>
       <c r="J5" t="s">
         <v>9</v>
@@ -572,28 +572,28 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>39605.292</v>
+        <v>49385.5195</v>
       </c>
       <c r="C6">
-        <v>160197.7818153145</v>
+        <v>193850.697720596</v>
       </c>
       <c r="D6">
         <v>1.999999997</v>
       </c>
       <c r="E6">
-        <v>-78344.05278555595</v>
+        <v>-395364.8421912249</v>
       </c>
       <c r="F6">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G6">
-        <v>34548288.1568762</v>
+        <v>36950421.4232691</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>24260947.4241898</v>
+        <v>24156638.5693997</v>
       </c>
       <c r="J6" t="s">
         <v>9</v>
@@ -604,28 +604,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>220800.977873</v>
-      </c>
-      <c r="C7">
-        <v>434350.8037123537</v>
+        <v>279246.515913</v>
       </c>
       <c r="D7">
-        <v>2.999999987</v>
+        <v>4.999999985</v>
       </c>
       <c r="E7">
-        <v>20415706.04726911</v>
+        <v>28271438.20374005</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
-      <c r="G7">
-        <v>113868022.405147</v>
-      </c>
       <c r="H7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>122626580.181268</v>
+        <v>132559336.26135</v>
       </c>
       <c r="J7" t="s">
         <v>9</v>
@@ -636,28 +630,28 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>94029.88</v>
+        <v>118411.95</v>
       </c>
       <c r="C8">
-        <v>222132.6624396211</v>
+        <v>268796.303622337</v>
       </c>
       <c r="D8">
         <v>2.999999996</v>
       </c>
       <c r="E8">
-        <v>-1109004.899437587</v>
+        <v>-1277732.629437586</v>
       </c>
       <c r="F8">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G8">
-        <v>67854770.3288119</v>
+        <v>65867510.0509068</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I8">
-        <v>48816684.3826114</v>
+        <v>49886784.6835634</v>
       </c>
       <c r="J8" t="s">
         <v>9</v>
@@ -668,28 +662,28 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>193462.078507</v>
+        <v>226907.941727</v>
       </c>
       <c r="C9">
-        <v>258928.6813138488</v>
+        <v>313322.1007418785</v>
       </c>
       <c r="D9">
         <v>0.999999992</v>
       </c>
       <c r="E9">
-        <v>5161194.792964611</v>
+        <v>4720467.70784786</v>
       </c>
       <c r="F9">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G9">
-        <v>84748836.86864419</v>
+        <v>89465155.19588719</v>
       </c>
       <c r="H9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I9">
-        <v>68407346.0580954</v>
+        <v>70133146.86166421</v>
       </c>
       <c r="J9" t="s">
         <v>9</v>
@@ -700,28 +694,28 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>11950.2</v>
+        <v>27423.9139</v>
       </c>
       <c r="C10">
-        <v>136981.808504433</v>
+        <v>165757.7205671078</v>
       </c>
       <c r="D10">
-        <v>-1E-09</v>
+        <v>1.999999997</v>
       </c>
       <c r="E10">
-        <v>7190534.138944714</v>
+        <v>9447875.952797854</v>
       </c>
       <c r="F10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10">
-        <v>62213266.2439621</v>
+        <v>66879630.3622337</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I10">
-        <v>45230851.5975286</v>
+        <v>48056588.2187911</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
@@ -732,28 +726,28 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>191104.36334</v>
+        <v>224764.57836</v>
       </c>
       <c r="C11">
-        <v>233929.1678262628</v>
+        <v>283070.9132577037</v>
       </c>
       <c r="D11">
-        <v>1.999999991</v>
+        <v>-7E-09</v>
       </c>
       <c r="E11">
-        <v>9606825.02718243</v>
+        <v>12137737.88375509</v>
       </c>
       <c r="F11">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G11">
-        <v>64193977.025966</v>
+        <v>66004327.5546375</v>
       </c>
       <c r="H11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I11">
-        <v>60222733.0647059</v>
+        <v>62031125.3162258</v>
       </c>
       <c r="J11" t="s">
         <v>9</v>
@@ -764,28 +758,28 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>246358.4988750001</v>
+        <v>311633.7437350002</v>
       </c>
       <c r="C12">
-        <v>555331.656099053</v>
+        <v>627191.375118786</v>
       </c>
       <c r="D12">
         <v>-6E-09</v>
       </c>
       <c r="E12">
-        <v>14710453.94383574</v>
+        <v>20709427.39561249</v>
       </c>
       <c r="F12">
         <v>13</v>
       </c>
       <c r="G12">
-        <v>114243500.633576</v>
+        <v>120520866.772065</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I12">
-        <v>109326642.258857</v>
+        <v>111336706.643765</v>
       </c>
       <c r="J12" t="s">
         <v>9</v>
@@ -796,28 +790,28 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>101273.089932</v>
+        <v>110810.418692</v>
       </c>
       <c r="C13">
-        <v>251750.3507649039</v>
+        <v>304635.8107719819</v>
       </c>
       <c r="D13">
-        <v>2.999999984</v>
+        <v>1.999999985</v>
       </c>
       <c r="E13">
-        <v>12376461.17479195</v>
+        <v>14425098.89858874</v>
       </c>
       <c r="F13">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G13">
-        <v>92999378.96092241</v>
+        <v>95636875.7250993</v>
       </c>
       <c r="H13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I13">
-        <v>87404677.8380408</v>
+        <v>86620609.10685951</v>
       </c>
       <c r="J13" t="s">
         <v>9</v>
@@ -828,28 +822,28 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>113426.696207</v>
+        <v>136114.660307</v>
       </c>
       <c r="C14">
-        <v>234198.0993802445</v>
+        <v>283396.3395450573</v>
       </c>
       <c r="D14">
         <v>2.99999999</v>
       </c>
       <c r="E14">
-        <v>-589065.4310853328</v>
+        <v>163899.529774836</v>
       </c>
       <c r="F14">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G14">
-        <v>82639288.8756644</v>
+        <v>88162403.00945599</v>
       </c>
       <c r="H14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I14">
-        <v>57888711.2816055</v>
+        <v>58912880.5055408</v>
       </c>
       <c r="J14" t="s">
         <v>9</v>
@@ -860,28 +854,28 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>77437.50004100001</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>222132.6624396211</v>
+        <v>188157.4125356359</v>
       </c>
       <c r="D15">
-        <v>4.99999999</v>
+        <v>3.999999995</v>
       </c>
       <c r="E15">
-        <v>-1734438.653159759</v>
+        <v>3416998.1415625</v>
       </c>
       <c r="F15">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G15">
-        <v>54673196.3605466</v>
+        <v>44799383.9370562</v>
       </c>
       <c r="H15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I15">
-        <v>42846879.675681</v>
+        <v>8130155.51005326</v>
       </c>
       <c r="J15" t="s">
         <v>9</v>
@@ -892,28 +886,28 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>198236.952662</v>
+        <v>112651.161581</v>
       </c>
       <c r="C16">
-        <v>491502.5759892353</v>
+        <v>268796.303622337</v>
       </c>
       <c r="D16">
-        <v>0.999999993</v>
+        <v>4.99999999</v>
       </c>
       <c r="E16">
-        <v>5633652.590549201</v>
+        <v>-688448.9842057356</v>
       </c>
       <c r="F16">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G16">
-        <v>136591527.386474</v>
+        <v>57183396.5740578</v>
       </c>
       <c r="H16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I16">
-        <v>118249454.369191</v>
+        <v>44025324.5983992</v>
       </c>
       <c r="J16" t="s">
         <v>9</v>
@@ -924,28 +918,28 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>135509.8325430001</v>
+        <v>250751.614062</v>
       </c>
       <c r="C17">
-        <v>379932.3532480986</v>
+        <v>594753.0371976423</v>
       </c>
       <c r="D17">
-        <v>1.999999995</v>
+        <v>0.999999993</v>
       </c>
       <c r="E17">
-        <v>7274574.737954758</v>
+        <v>8032350.7650893</v>
       </c>
       <c r="F17">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G17">
-        <v>111937845.769439</v>
+        <v>140443579.463008</v>
       </c>
       <c r="H17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I17">
-        <v>110770759.530826</v>
+        <v>123566046.138903</v>
       </c>
       <c r="J17" t="s">
         <v>9</v>
@@ -956,28 +950,28 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>149829.159721</v>
+        <v>166713.6957030001</v>
       </c>
       <c r="C18">
-        <v>203137.5237481997</v>
+        <v>459745.1408452092</v>
       </c>
       <c r="D18">
-        <v>2.999999992</v>
+        <v>1.999999995</v>
       </c>
       <c r="E18">
-        <v>6332936.341271805</v>
+        <v>10540497.57212998</v>
       </c>
       <c r="F18">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G18">
-        <v>55744247.9438409</v>
+        <v>113929898.858352</v>
       </c>
       <c r="H18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I18">
-        <v>67263412.6694053</v>
+        <v>116424007.92435</v>
       </c>
       <c r="J18" t="s">
         <v>9</v>
@@ -988,28 +982,28 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>98283.26676200001</v>
+        <v>176563.898581</v>
       </c>
       <c r="C19">
-        <v>117063.9565028025</v>
+        <v>245810.8362400445</v>
       </c>
       <c r="D19">
-        <v>0.999999996</v>
+        <v>1.999999993</v>
       </c>
       <c r="E19">
-        <v>5938551.258625419</v>
+        <v>9630383.649145005</v>
       </c>
       <c r="F19">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G19">
-        <v>31985998.5410285</v>
+        <v>57316305.532588</v>
       </c>
       <c r="H19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I19">
-        <v>33058990.9965707</v>
+        <v>71559483.5310411</v>
       </c>
       <c r="J19" t="s">
         <v>9</v>
@@ -1020,28 +1014,28 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>86881.400022</v>
+        <v>118179.140522</v>
       </c>
       <c r="C20">
-        <v>163164.407404487</v>
+        <v>141655.7045225727</v>
       </c>
       <c r="D20">
-        <v>1.999999992</v>
+        <v>0.999999996</v>
       </c>
       <c r="E20">
-        <v>13894412.95411212</v>
+        <v>12709479.21787969</v>
       </c>
       <c r="F20">
         <v>9</v>
       </c>
       <c r="G20">
-        <v>41611024.042152</v>
+        <v>32909016.7893645</v>
       </c>
       <c r="H20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I20">
-        <v>50424698.0806562</v>
+        <v>39169642.8058211</v>
       </c>
       <c r="J20" t="s">
         <v>9</v>
@@ -1052,28 +1046,28 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>65462.60676</v>
+        <v>98478.38504199999</v>
       </c>
       <c r="C21">
-        <v>222132.6624396211</v>
+        <v>197440.5254561626</v>
       </c>
       <c r="D21">
-        <v>0.9999999939999999</v>
+        <v>1.999999992</v>
       </c>
       <c r="E21">
-        <v>6837769.251800663</v>
+        <v>13483984.57258214</v>
       </c>
       <c r="F21">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="G21">
-        <v>66548837.2412698</v>
+        <v>43264457.1595386</v>
       </c>
       <c r="H21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I21">
-        <v>65044666.3251653</v>
+        <v>50942225.2829145</v>
       </c>
       <c r="J21" t="s">
         <v>9</v>
@@ -1084,28 +1078,28 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>139068.236665</v>
+        <v>82825.84376</v>
       </c>
       <c r="C22">
-        <v>266559.1949275453</v>
+        <v>268796.303622337</v>
       </c>
       <c r="D22">
-        <v>1.99999999</v>
+        <v>0.9999999939999999</v>
       </c>
       <c r="E22">
-        <v>4582130.69898687</v>
+        <v>8735829.482966226</v>
       </c>
       <c r="F22">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G22">
-        <v>65163345.6463628</v>
+        <v>69444871.20746569</v>
       </c>
       <c r="H22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I22">
-        <v>58549638.9094989</v>
+        <v>66609639.7023026</v>
       </c>
       <c r="J22" t="s">
         <v>9</v>
@@ -1116,28 +1110,28 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>152063.369487</v>
+        <v>204415.709125</v>
       </c>
       <c r="C23">
-        <v>360495.0254411163</v>
+        <v>268796.303622337</v>
       </c>
       <c r="D23">
-        <v>2.999999993</v>
+        <v>2.999999989</v>
       </c>
       <c r="E23">
-        <v>2248115.228082923</v>
+        <v>6345431.665514652</v>
       </c>
       <c r="F23">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G23">
-        <v>100183727.444379</v>
+        <v>68765064.9344134</v>
       </c>
       <c r="H23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I23">
-        <v>92243199.832435</v>
+        <v>61783181.6933618</v>
       </c>
       <c r="J23" t="s">
         <v>9</v>
@@ -1148,28 +1142,28 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>412718.3925389999</v>
+        <v>194163.913047</v>
       </c>
       <c r="C24">
-        <v>466478.5911232043</v>
+        <v>436224.5932164576</v>
       </c>
       <c r="D24">
-        <v>13.999999985</v>
+        <v>2.999999993</v>
       </c>
       <c r="E24">
-        <v>72464620.03095177</v>
+        <v>4440189.221211218</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G24">
-        <v>111735001.751631</v>
+        <v>103009033.986665</v>
       </c>
       <c r="H24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I24">
-        <v>150519833.488363</v>
+        <v>95985094.22961649</v>
       </c>
       <c r="J24" t="s">
         <v>9</v>
@@ -1180,28 +1174,28 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>146622.4872259999</v>
+        <v>565179.4984789999</v>
       </c>
       <c r="C25">
-        <v>466478.5911232043</v>
+        <v>564472.2376069077</v>
       </c>
       <c r="D25">
-        <v>9.999999989000001</v>
+        <v>14.999999984</v>
       </c>
       <c r="E25">
-        <v>9269254.680725597</v>
+        <v>79762159.1690679</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>117257122.942305</v>
+        <v>118207994.076012</v>
       </c>
       <c r="H25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I25">
-        <v>121356904.654824</v>
+        <v>160152293.874123</v>
       </c>
       <c r="J25" t="s">
         <v>9</v>
@@ -1212,28 +1206,28 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>114254.301774</v>
+        <v>210427.546306</v>
       </c>
       <c r="C26">
-        <v>466478.5911232043</v>
+        <v>564472.2376069077</v>
       </c>
       <c r="D26">
-        <v>2.99999999</v>
+        <v>7.999999991</v>
       </c>
       <c r="E26">
-        <v>-5036239.013481954</v>
+        <v>12697706.55173514</v>
       </c>
       <c r="F26">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="G26">
-        <v>88945246.3752941</v>
+        <v>125055714.234396</v>
       </c>
       <c r="H26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I26">
-        <v>74110425.6481806</v>
+        <v>125474356.64008</v>
       </c>
       <c r="J26" t="s">
         <v>9</v>
@@ -1244,28 +1238,28 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>215804.1175</v>
+        <v>201118.835714</v>
       </c>
       <c r="C27">
-        <v>888530.649758485</v>
+        <v>447993.8393705615</v>
       </c>
       <c r="D27">
-        <v>2.999999987</v>
+        <v>3.999999989</v>
       </c>
       <c r="E27">
-        <v>60383311.36380333</v>
+        <v>-5273485.495753588</v>
       </c>
       <c r="F27">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G27">
-        <v>121101556.210078</v>
+        <v>93543166.2384655</v>
       </c>
       <c r="H27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I27">
-        <v>159377098.203532</v>
+        <v>75236861.7829894</v>
       </c>
       <c r="J27" t="s">
         <v>9</v>
@@ -1276,28 +1270,28 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>114536.919981</v>
+        <v>309371.4254999999</v>
       </c>
       <c r="C28">
-        <v>148088.4416264141</v>
+        <v>627191.375118786</v>
       </c>
       <c r="D28">
-        <v>-1.000000003</v>
+        <v>2.999999987</v>
       </c>
       <c r="E28">
-        <v>7525058.468946218</v>
+        <v>67157403.89008105</v>
       </c>
       <c r="F28">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="G28">
-        <v>32235854.4869002</v>
+        <v>128532347.967239</v>
       </c>
       <c r="H28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I28">
-        <v>25674795.9708921</v>
+        <v>168993135.734353</v>
       </c>
       <c r="J28" t="s">
         <v>9</v>
@@ -1308,28 +1302,28 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>2428.12</v>
+        <v>149959.284461</v>
       </c>
       <c r="C29">
-        <v>148331.2794586246</v>
+        <v>179197.5357482248</v>
       </c>
       <c r="D29">
-        <v>-1E-09</v>
+        <v>0.999999995</v>
       </c>
       <c r="E29">
-        <v>749228.672174304</v>
+        <v>9585279.296527943</v>
       </c>
       <c r="F29">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="G29">
-        <v>19812515.4550101</v>
+        <v>35664507.8665033</v>
       </c>
       <c r="H29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I29">
-        <v>3705464.75801017</v>
+        <v>29011722.1974944</v>
       </c>
       <c r="J29" t="s">
         <v>9</v>
@@ -1340,28 +1334,28 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>93625.051028</v>
+        <v>3202.44</v>
       </c>
       <c r="C30">
-        <v>213473.9808577294</v>
+        <v>179491.3867783297</v>
       </c>
       <c r="D30">
-        <v>12.999999977</v>
+        <v>-1E-09</v>
       </c>
       <c r="E30">
-        <v>9771576.246647231</v>
+        <v>749228.672174304</v>
       </c>
       <c r="F30">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="G30">
-        <v>47406415.5477206</v>
+        <v>23540432.1257414</v>
       </c>
       <c r="H30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I30">
-        <v>47431457.3887473</v>
+        <v>3769167.73774433</v>
       </c>
       <c r="J30" t="s">
         <v>9</v>
@@ -1372,28 +1366,22 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>46722.736791</v>
-      </c>
-      <c r="C31">
-        <v>133279.5974637727</v>
+        <v>113004.929588</v>
       </c>
       <c r="D31">
-        <v>0.9999999979999999</v>
+        <v>10.999999979</v>
       </c>
       <c r="E31">
-        <v>27337898.79912266</v>
+        <v>11784528.38437979</v>
       </c>
       <c r="F31">
-        <v>10</v>
-      </c>
-      <c r="G31">
-        <v>26191918.7607475</v>
+        <v>7</v>
       </c>
       <c r="H31">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I31">
-        <v>33729840.7642913</v>
+        <v>54015049.9983958</v>
       </c>
       <c r="J31" t="s">
         <v>9</v>
@@ -1404,28 +1392,28 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>174161.1991100001</v>
+        <v>61390.669431</v>
       </c>
       <c r="C32">
-        <v>427877.2368349028</v>
+        <v>161277.7821734023</v>
       </c>
       <c r="D32">
-        <v>1.999999993</v>
+        <v>3.999999995</v>
       </c>
       <c r="E32">
-        <v>5649693.337566338</v>
+        <v>49143446.77005175</v>
       </c>
       <c r="F32">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G32">
-        <v>126063641.949974</v>
+        <v>40319445.5433506</v>
       </c>
       <c r="H32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I32">
-        <v>126246260.677972</v>
+        <v>62035701.8863961</v>
       </c>
       <c r="J32" t="s">
         <v>9</v>
@@ -1436,31 +1424,31 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>342449.6492389999</v>
+        <v>206845.6237900001</v>
       </c>
       <c r="C33">
-        <v>483878.983014308</v>
+        <v>517761.8563709559</v>
       </c>
       <c r="D33">
-        <v>2.999999987</v>
+        <v>2.999999992</v>
       </c>
       <c r="E33">
-        <v>7598263.076584458</v>
+        <v>6069764.464888243</v>
       </c>
       <c r="F33">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G33">
-        <v>242639591.721809</v>
+        <v>128307078.614489</v>
       </c>
       <c r="H33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I33">
-        <v>218982271.955886</v>
+        <v>131135133.148493</v>
       </c>
       <c r="J33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1468,28 +1456,19 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>1084893.102502</v>
-      </c>
-      <c r="C34">
-        <v>1644495.303231283</v>
+        <v>437041.5331989997</v>
       </c>
       <c r="D34">
-        <v>0.9999999899999999</v>
+        <v>4.999999985</v>
       </c>
       <c r="E34">
-        <v>-4449809.823869223</v>
-      </c>
-      <c r="F34">
-        <v>14</v>
-      </c>
-      <c r="G34">
-        <v>454820355.769472</v>
+        <v>14129465.69103084</v>
       </c>
       <c r="H34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I34">
-        <v>413005803.024958</v>
+        <v>228903868.273275</v>
       </c>
       <c r="J34" t="s">
         <v>10</v>
@@ -1500,28 +1479,25 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>118740.4024419999</v>
+        <v>1427756.390602</v>
       </c>
       <c r="C35">
-        <v>331876.1936546037</v>
+        <v>1989956.15493068</v>
       </c>
       <c r="D35">
-        <v>3.999999994</v>
+        <v>-9E-09</v>
       </c>
       <c r="E35">
-        <v>11390899.35385293</v>
-      </c>
-      <c r="F35">
-        <v>30</v>
+        <v>-7245394.153791307</v>
       </c>
       <c r="G35">
-        <v>155529138.301549</v>
+        <v>462914368.036666</v>
       </c>
       <c r="H35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I35">
-        <v>135113126.981393</v>
+        <v>419200040.408371</v>
       </c>
       <c r="J35" t="s">
         <v>10</v>
@@ -1532,28 +1508,25 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>248119.1473</v>
+        <v>160878.3722619999</v>
       </c>
       <c r="C36">
-        <v>555331.656099053</v>
+        <v>401593.7734454345</v>
       </c>
       <c r="D36">
-        <v>-7E-09</v>
+        <v>4.999999993</v>
       </c>
       <c r="E36">
-        <v>-56271.18975162401</v>
-      </c>
-      <c r="F36">
-        <v>29</v>
+        <v>15674217.66116987</v>
       </c>
       <c r="G36">
-        <v>171724286.932034</v>
+        <v>162971737.218567</v>
       </c>
       <c r="H36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I36">
-        <v>155504634.128037</v>
+        <v>140937442.588492</v>
       </c>
       <c r="J36" t="s">
         <v>10</v>
@@ -1564,28 +1537,25 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>437976.720448</v>
+        <v>547208.544608</v>
       </c>
       <c r="C37">
-        <v>592282.587796188</v>
+        <v>716704.011697341</v>
       </c>
       <c r="D37">
         <v>1.99999999</v>
       </c>
       <c r="E37">
-        <v>17558559.17956881</v>
-      </c>
-      <c r="F37">
-        <v>13</v>
+        <v>19674320.38476177</v>
       </c>
       <c r="G37">
-        <v>161152479.158127</v>
+        <v>165949842.129764</v>
       </c>
       <c r="H37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I37">
-        <v>161370812.304825</v>
+        <v>165646739.058223</v>
       </c>
       <c r="J37" t="s">
         <v>10</v>
@@ -1596,28 +1566,25 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>567781.735633</v>
+        <v>659069.2998729999</v>
       </c>
       <c r="C38">
-        <v>681916.665005233</v>
+        <v>825167.6134377619</v>
       </c>
       <c r="D38">
-        <v>2.999999981</v>
+        <v>7.999999976</v>
       </c>
       <c r="E38">
-        <v>23522190.28766121</v>
-      </c>
-      <c r="F38">
-        <v>2</v>
+        <v>27574170.14620421</v>
       </c>
       <c r="G38">
-        <v>189958251.959003</v>
+        <v>195397061.094805</v>
       </c>
       <c r="H38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I38">
-        <v>193464867.760403</v>
+        <v>200151254.904617</v>
       </c>
       <c r="J38" t="s">
         <v>10</v>
@@ -1628,28 +1595,19 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>988306.2640580011</v>
-      </c>
-      <c r="C39">
-        <v>1642028.705125444</v>
+        <v>1166441.761158001</v>
       </c>
       <c r="D39">
-        <v>0.999999979</v>
+        <v>-2E-08</v>
       </c>
       <c r="E39">
-        <v>10411129.78304642</v>
-      </c>
-      <c r="F39">
-        <v>6</v>
-      </c>
-      <c r="G39">
-        <v>352891766.084769</v>
+        <v>9073580.796574228</v>
       </c>
       <c r="H39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I39">
-        <v>370552413.68817</v>
+        <v>348565330.671247</v>
       </c>
       <c r="J39" t="s">
         <v>10</v>
@@ -1660,28 +1618,25 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>263443.4489659996</v>
+        <v>324307.9065659997</v>
       </c>
       <c r="C40">
-        <v>481287.4352858456</v>
+        <v>582391.9911817291</v>
       </c>
       <c r="D40">
-        <v>-5E-09</v>
+        <v>0.9999999939999999</v>
       </c>
       <c r="E40">
-        <v>1286021.821924305</v>
-      </c>
-      <c r="F40">
-        <v>27</v>
+        <v>2744269.595138839</v>
       </c>
       <c r="G40">
-        <v>259507877.66895</v>
+        <v>264508335.976307</v>
       </c>
       <c r="H40">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I40">
-        <v>244713549.408212</v>
+        <v>251447120.831897</v>
       </c>
       <c r="J40" t="s">
         <v>10</v>
@@ -1692,28 +1647,25 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>208687.60489</v>
+        <v>261352.09457</v>
       </c>
       <c r="C41">
-        <v>536290.34415543</v>
+        <v>648949.418757872</v>
       </c>
       <c r="D41">
-        <v>-5.000000006</v>
+        <v>-4.000000007</v>
       </c>
       <c r="E41">
-        <v>20200258.82331599</v>
-      </c>
-      <c r="F41">
-        <v>34</v>
+        <v>22689221.6004031</v>
       </c>
       <c r="G41">
-        <v>176851462.773747</v>
+        <v>180773023.234012</v>
       </c>
       <c r="H41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I41">
-        <v>127742527.064115</v>
+        <v>130811153.108373</v>
       </c>
       <c r="J41" t="s">
         <v>10</v>
@@ -1724,28 +1676,19 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>385319.071562</v>
-      </c>
-      <c r="C42">
-        <v>463272.4787591225</v>
+        <v>485061.0454419998</v>
       </c>
       <c r="D42">
-        <v>-1.3E-08</v>
+        <v>1.999999985</v>
       </c>
       <c r="E42">
-        <v>16043594.10435642</v>
-      </c>
-      <c r="F42">
-        <v>11</v>
-      </c>
-      <c r="G42">
-        <v>136491990.832644</v>
+        <v>21084562.53407755</v>
       </c>
       <c r="H42">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I42">
-        <v>146174171.479538</v>
+        <v>152146785.390455</v>
       </c>
       <c r="J42" t="s">
         <v>10</v>
@@ -1756,28 +1699,25 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>360442.4835979996</v>
+        <v>456089.5878179997</v>
       </c>
       <c r="C43">
-        <v>944687.927674478</v>
+        <v>1143139.510627199</v>
       </c>
       <c r="D43">
-        <v>0.999999983</v>
+        <v>-2.000000014</v>
       </c>
       <c r="E43">
-        <v>9992080.358713957</v>
-      </c>
-      <c r="F43">
-        <v>28</v>
+        <v>8365578.784704198</v>
       </c>
       <c r="G43">
-        <v>262534484.277137</v>
+        <v>269938285.450157</v>
       </c>
       <c r="H43">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I43">
-        <v>238809887.483227</v>
+        <v>240470886.97798</v>
       </c>
       <c r="J43" t="s">
         <v>10</v>
@@ -1788,28 +1728,25 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>790044.279498</v>
+        <v>1045518.143118</v>
       </c>
       <c r="C44">
-        <v>1545840.316135137</v>
+        <v>1870576.611309708</v>
       </c>
       <c r="D44">
-        <v>5.99999996</v>
+        <v>8.999999957</v>
       </c>
       <c r="E44">
-        <v>56527781.34839144</v>
-      </c>
-      <c r="F44">
-        <v>10</v>
+        <v>67699177.56819198</v>
       </c>
       <c r="G44">
-        <v>429729879.613681</v>
+        <v>453930494.313569</v>
       </c>
       <c r="H44">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I44">
-        <v>379106601.089066</v>
+        <v>398308822.759385</v>
       </c>
       <c r="J44" t="s">
         <v>10</v>
@@ -1820,28 +1757,25 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>477472.6346250001</v>
+        <v>595891.9738200001</v>
       </c>
       <c r="C45">
-        <v>599758.188586978</v>
+        <v>725750.019780311</v>
       </c>
       <c r="D45">
-        <v>0.999999959</v>
+        <v>-1.000000039</v>
       </c>
       <c r="E45">
-        <v>26231645.62264343</v>
-      </c>
-      <c r="F45">
-        <v>4</v>
+        <v>30991267.53152352</v>
       </c>
       <c r="G45">
-        <v>326048382.36872</v>
+        <v>349123366.348481</v>
       </c>
       <c r="H45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I45">
-        <v>344973039.259336</v>
+        <v>346315867.113864</v>
       </c>
       <c r="J45" t="s">
         <v>10</v>
@@ -1852,28 +1786,25 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>688774.4320500001</v>
+        <v>901451.858009999</v>
       </c>
       <c r="C46">
-        <v>2432352.653713851</v>
+        <v>2943319.52466459</v>
       </c>
       <c r="D46">
-        <v>10.999999979</v>
+        <v>4.999999985</v>
       </c>
       <c r="E46">
-        <v>27834409.96992368</v>
-      </c>
-      <c r="F46">
-        <v>25</v>
+        <v>37792529.97965544</v>
       </c>
       <c r="G46">
-        <v>809860929.883302</v>
+        <v>871844868.1560791</v>
       </c>
       <c r="H46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I46">
-        <v>338720929.045818</v>
+        <v>356571751.166594</v>
       </c>
       <c r="J46" t="s">
         <v>10</v>
@@ -1884,28 +1815,25 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>482243.4961860002</v>
+        <v>332567.650706</v>
       </c>
       <c r="C47">
-        <v>555331.656099053</v>
+        <v>447993.8393705615</v>
       </c>
       <c r="D47">
         <v>-1.000000008</v>
       </c>
       <c r="E47">
-        <v>-2184469.685127309</v>
-      </c>
-      <c r="F47">
-        <v>16</v>
+        <v>1489812.729699546</v>
       </c>
       <c r="G47">
-        <v>447166847.816603</v>
+        <v>392707751.013488</v>
       </c>
       <c r="H47">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I47">
-        <v>416364724.092742</v>
+        <v>351708377.004988</v>
       </c>
       <c r="J47" t="s">
         <v>10</v>
@@ -1916,28 +1844,25 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>309259.542458</v>
+        <v>389937.957858</v>
       </c>
       <c r="C48">
-        <v>566873.002004728</v>
+        <v>685956.607590682</v>
       </c>
       <c r="D48">
         <v>0.999999991</v>
       </c>
       <c r="E48">
-        <v>-1955964.196263</v>
-      </c>
-      <c r="F48">
-        <v>26</v>
+        <v>4327483.929702809</v>
       </c>
       <c r="G48">
-        <v>125273801.741904</v>
+        <v>127932972.017863</v>
       </c>
       <c r="H48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I48">
-        <v>131088981.594749</v>
+        <v>139025695.080742</v>
       </c>
       <c r="J48" t="s">
         <v>10</v>
@@ -1948,28 +1873,25 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>246383.6611919999</v>
+        <v>330437.0770120001</v>
       </c>
       <c r="C49">
-        <v>646465.681693802</v>
+        <v>782269.404911224</v>
       </c>
       <c r="D49">
         <v>0.9999999899999999</v>
       </c>
       <c r="E49">
-        <v>5440803.371100672</v>
-      </c>
-      <c r="F49">
-        <v>31</v>
+        <v>9157319.962886602</v>
       </c>
       <c r="G49">
-        <v>183105704.555881</v>
+        <v>188896780.837437</v>
       </c>
       <c r="H49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I49">
-        <v>165254880.798772</v>
+        <v>173186776.487825</v>
       </c>
       <c r="J49" t="s">
         <v>10</v>
@@ -1980,28 +1902,19 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>535496.432444</v>
-      </c>
-      <c r="C50">
-        <v>1089501.103668586</v>
+        <v>704143.3872839999</v>
       </c>
       <c r="D50">
-        <v>8.999999969999999</v>
+        <v>11.999999967</v>
       </c>
       <c r="E50">
-        <v>6563757.079816269</v>
-      </c>
-      <c r="F50">
-        <v>15</v>
-      </c>
-      <c r="G50">
-        <v>303399679.582023</v>
+        <v>99004889.16466613</v>
       </c>
       <c r="H50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I50">
-        <v>356548374.653075</v>
+        <v>375049738.363188</v>
       </c>
       <c r="J50" t="s">
         <v>10</v>
@@ -2012,28 +1925,25 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>460794.793745</v>
+        <v>738857.865405001</v>
       </c>
       <c r="C51">
-        <v>1236279.332807711</v>
+        <v>1495985.827810116</v>
       </c>
       <c r="D51">
         <v>-1.4E-08</v>
       </c>
       <c r="E51">
-        <v>-13092376.68955193</v>
-      </c>
-      <c r="F51">
-        <v>33</v>
+        <v>-4070848.855628334</v>
       </c>
       <c r="G51">
-        <v>343569465.32054</v>
+        <v>353258554.43773</v>
       </c>
       <c r="H51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I51">
-        <v>281832417.174738</v>
+        <v>294729975.30405</v>
       </c>
       <c r="J51" t="s">
         <v>10</v>
@@ -2044,28 +1954,25 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>324686.5495939998</v>
+        <v>1316923.272999999</v>
       </c>
       <c r="C52">
-        <v>1222550.793826734</v>
+        <v>1209583.366300517</v>
       </c>
       <c r="D52">
-        <v>-1.4E-08</v>
+        <v>0.999999984</v>
       </c>
       <c r="E52">
-        <v>4310762.567984672</v>
-      </c>
-      <c r="F52">
-        <v>35</v>
+        <v>20948099.12176</v>
       </c>
       <c r="G52">
-        <v>339754266.677222</v>
+        <v>393097049.230891</v>
       </c>
       <c r="H52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I52">
-        <v>279762989.445939</v>
+        <v>399360239.004852</v>
       </c>
       <c r="J52" t="s">
         <v>10</v>
@@ -2076,28 +1983,25 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>1006876.154626</v>
+        <v>399500.4786539997</v>
       </c>
       <c r="C53">
-        <v>1937041.709484575</v>
+        <v>1479373.320258577</v>
       </c>
       <c r="D53">
-        <v>2.999999985</v>
+        <v>0.999999985</v>
       </c>
       <c r="E53">
-        <v>21602894.52623686</v>
-      </c>
-      <c r="F53">
-        <v>5</v>
+        <v>2406525.909258162</v>
       </c>
       <c r="G53">
-        <v>478768141.499364</v>
+        <v>349335762.370402</v>
       </c>
       <c r="H53">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I53">
-        <v>452684032.000811</v>
+        <v>285022400.390091</v>
       </c>
       <c r="J53" t="s">
         <v>10</v>
@@ -2108,28 +2012,25 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>913708.949974</v>
+        <v>1664608.373266002</v>
       </c>
       <c r="C54">
-        <v>2113783.047100886</v>
+        <v>2343958.091319741</v>
       </c>
       <c r="D54">
-        <v>-2.000000032</v>
+        <v>5.999999982</v>
       </c>
       <c r="E54">
-        <v>23928936.56337655</v>
-      </c>
-      <c r="F54">
-        <v>20</v>
+        <v>36880788.4355883</v>
       </c>
       <c r="G54">
-        <v>540727346.360548</v>
+        <v>490132517.48139</v>
       </c>
       <c r="H54">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I54">
-        <v>490312957.119861</v>
+        <v>475500342.421061</v>
       </c>
       <c r="J54" t="s">
         <v>10</v>
@@ -2140,28 +2041,19 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>261016.1885250002</v>
-      </c>
-      <c r="C55">
-        <v>633466.449891085</v>
+        <v>1192790.478853999</v>
       </c>
       <c r="D55">
-        <v>0.999999991</v>
+        <v>-5.000000029</v>
       </c>
       <c r="E55">
-        <v>-3515175.529913017</v>
-      </c>
-      <c r="F55">
-        <v>32</v>
-      </c>
-      <c r="G55">
-        <v>176044199.383173</v>
+        <v>24041690.26878395</v>
       </c>
       <c r="H55">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I55">
-        <v>150532692.127773</v>
+        <v>499237175.937533</v>
       </c>
       <c r="J55" t="s">
         <v>10</v>
@@ -2172,28 +2064,25 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>479256.598085</v>
+        <v>295237.1833050001</v>
       </c>
       <c r="C56">
-        <v>555331.656099053</v>
+        <v>766539.41086116</v>
       </c>
       <c r="D56">
-        <v>3.99999999</v>
+        <v>0.999999991</v>
       </c>
       <c r="E56">
-        <v>42433780.57660335</v>
-      </c>
-      <c r="F56">
-        <v>7</v>
+        <v>-2412282.298719347</v>
       </c>
       <c r="G56">
-        <v>270736454.08915</v>
+        <v>181008866.249681</v>
       </c>
       <c r="H56">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I56">
-        <v>230576273.740458</v>
+        <v>150776833.048063</v>
       </c>
       <c r="J56" t="s">
         <v>10</v>
@@ -2204,28 +2093,25 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>778900.249476</v>
+        <v>559147.208685</v>
       </c>
       <c r="C57">
-        <v>888530.649758485</v>
+        <v>671990.759055843</v>
       </c>
       <c r="D57">
-        <v>1.999999983</v>
+        <v>4.999999989</v>
       </c>
       <c r="E57">
-        <v>2644912.85419981</v>
-      </c>
-      <c r="F57">
-        <v>8</v>
+        <v>46342348.84790082</v>
       </c>
       <c r="G57">
-        <v>432969481.648568</v>
+        <v>280524877.955404</v>
       </c>
       <c r="H57">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I57">
-        <v>382137386.556102</v>
+        <v>238815037.368466</v>
       </c>
       <c r="J57" t="s">
         <v>10</v>
@@ -2236,28 +2122,25 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>834571.857233</v>
+        <v>948751.756936</v>
       </c>
       <c r="C58">
-        <v>888530.649758485</v>
+        <v>1075185.214489349</v>
       </c>
       <c r="D58">
-        <v>2.999999985</v>
+        <v>2.999999982</v>
       </c>
       <c r="E58">
-        <v>-21802401.92834045</v>
-      </c>
-      <c r="F58">
-        <v>9</v>
+        <v>19574394.36861564</v>
       </c>
       <c r="G58">
-        <v>425035273.063137</v>
+        <v>443866203.113601</v>
       </c>
       <c r="H58">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I58">
-        <v>365614916.690261</v>
+        <v>402289284.770169</v>
       </c>
       <c r="J58" t="s">
         <v>10</v>
@@ -2268,28 +2151,25 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>663830.596778</v>
+        <v>1030383.516133</v>
       </c>
       <c r="C59">
-        <v>888530.649758485</v>
+        <v>1075185.214489349</v>
       </c>
       <c r="D59">
-        <v>-1.1E-08</v>
+        <v>2.999999985</v>
       </c>
       <c r="E59">
-        <v>-19786388.21295691</v>
-      </c>
-      <c r="F59">
-        <v>23</v>
+        <v>-18291582.73189784</v>
       </c>
       <c r="G59">
-        <v>511977568.830259</v>
+        <v>435872490.965229</v>
       </c>
       <c r="H59">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I59">
-        <v>442562942.623248</v>
+        <v>372284378.690909</v>
       </c>
       <c r="J59" t="s">
         <v>10</v>
@@ -2300,28 +2180,25 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>660083.055313</v>
+        <v>867290.346103</v>
       </c>
       <c r="C60">
-        <v>888530.649758485</v>
+        <v>1075185.214489349</v>
       </c>
       <c r="D60">
-        <v>-1.2E-08</v>
+        <v>-1.1E-08</v>
       </c>
       <c r="E60">
-        <v>-15696735.21091129</v>
-      </c>
-      <c r="F60">
-        <v>18</v>
+        <v>-16088246.30951444</v>
       </c>
       <c r="G60">
-        <v>348064693.026605</v>
+        <v>523466821.060994</v>
       </c>
       <c r="H60">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I60">
-        <v>368121494.517524</v>
+        <v>464730008.847567</v>
       </c>
       <c r="J60" t="s">
         <v>10</v>
@@ -2332,28 +2209,25 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>671461.757014</v>
+        <v>830777.7814730001</v>
       </c>
       <c r="C61">
-        <v>888530.649758485</v>
+        <v>1075185.214489349</v>
       </c>
       <c r="D61">
-        <v>-3.000000012</v>
+        <v>-1.2E-08</v>
       </c>
       <c r="E61">
-        <v>10845217.55540248</v>
-      </c>
-      <c r="F61">
-        <v>12</v>
+        <v>-7755943.79286405</v>
       </c>
       <c r="G61">
-        <v>394767013.213565</v>
+        <v>347512645.701532</v>
       </c>
       <c r="H61">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I61">
-        <v>376644405.507436</v>
+        <v>403819992.292377</v>
       </c>
       <c r="J61" t="s">
         <v>10</v>
@@ -2364,28 +2238,25 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>366985.9410589999</v>
+        <v>847785.775594</v>
       </c>
       <c r="C62">
-        <v>629375.87691226</v>
+        <v>1075185.214489349</v>
       </c>
       <c r="D62">
-        <v>5.999999981</v>
+        <v>-2.000000013</v>
       </c>
       <c r="E62">
-        <v>13932522.606697</v>
-      </c>
-      <c r="F62">
-        <v>19</v>
+        <v>14885126.86672064</v>
       </c>
       <c r="G62">
-        <v>304844530.974725</v>
+        <v>405377230.617039</v>
       </c>
       <c r="H62">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I62">
-        <v>302836540.366495</v>
+        <v>390448045.247282</v>
       </c>
       <c r="J62" t="s">
         <v>10</v>
@@ -2396,28 +2267,25 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>343319.868218</v>
+        <v>463968.8240989997</v>
       </c>
       <c r="C63">
-        <v>419583.9179415065</v>
+        <v>761589.526929955</v>
       </c>
       <c r="D63">
-        <v>0.999999993</v>
+        <v>4.999999982</v>
       </c>
       <c r="E63">
-        <v>3515576.719620276</v>
-      </c>
-      <c r="F63">
-        <v>21</v>
+        <v>16970925.28966693</v>
       </c>
       <c r="G63">
-        <v>139478574.970946</v>
+        <v>310420875.883594</v>
       </c>
       <c r="H63">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I63">
-        <v>123456182.500676</v>
+        <v>313137532.893437</v>
       </c>
       <c r="J63" t="s">
         <v>10</v>
@@ -2428,28 +2296,25 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>2960490.443057</v>
+        <v>431734.2034979999</v>
       </c>
       <c r="C64">
-        <v>3909534.85893733</v>
+        <v>456771.5319966288</v>
       </c>
       <c r="D64">
-        <v>4.999999965</v>
+        <v>1.999999992</v>
       </c>
       <c r="E64">
-        <v>105191608.7962705</v>
-      </c>
-      <c r="F64">
-        <v>1</v>
+        <v>5398299.655918254</v>
       </c>
       <c r="G64">
-        <v>978062246.54098</v>
+        <v>143247730.662296</v>
       </c>
       <c r="H64">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I64">
-        <v>976899695.682322</v>
+        <v>127360244.329447</v>
       </c>
       <c r="J64" t="s">
         <v>10</v>
@@ -2460,28 +2325,19 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>1111768.868723</v>
-      </c>
-      <c r="C65">
-        <v>2013280.504745199</v>
+        <v>3632141.897297002</v>
       </c>
       <c r="D65">
-        <v>-1.000000022</v>
+        <v>4.999999965</v>
       </c>
       <c r="E65">
-        <v>6786338.936331124</v>
-      </c>
-      <c r="F65">
-        <v>17</v>
-      </c>
-      <c r="G65">
-        <v>555499019.115528</v>
+        <v>171051883.5710644</v>
       </c>
       <c r="H65">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I65">
-        <v>494532051.803154</v>
+        <v>1059393350.79388</v>
       </c>
       <c r="J65" t="s">
         <v>10</v>
@@ -2492,28 +2348,19 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>551058.582197</v>
-      </c>
-      <c r="C66">
-        <v>888530.649758485</v>
+        <v>1410706.602323</v>
       </c>
       <c r="D66">
-        <v>-1.1E-08</v>
+        <v>-2.3E-08</v>
       </c>
       <c r="E66">
-        <v>-8467177.808836775</v>
-      </c>
-      <c r="F66">
-        <v>24</v>
-      </c>
-      <c r="G66">
-        <v>633013935.80594</v>
+        <v>15754357.8058238</v>
       </c>
       <c r="H66">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I66">
-        <v>590503543.8303061</v>
+        <v>512437199.742186</v>
       </c>
       <c r="J66" t="s">
         <v>10</v>
@@ -2524,30 +2371,56 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>893372.738664002</v>
+        <v>708795.817177</v>
       </c>
       <c r="C67">
-        <v>1126548.389110266</v>
+        <v>940787.0626781799</v>
       </c>
       <c r="D67">
-        <v>0.999999982</v>
+        <v>-1.1E-08</v>
       </c>
       <c r="E67">
-        <v>11723347.76080601</v>
-      </c>
-      <c r="F67">
-        <v>3</v>
+        <v>-4735994.28343373</v>
       </c>
       <c r="G67">
-        <v>313074618.582843</v>
+        <v>642220644.6680959</v>
       </c>
       <c r="H67">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I67">
-        <v>291575394.45633</v>
+        <v>602016352.158518</v>
       </c>
       <c r="J67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>1117577.921944003</v>
+      </c>
+      <c r="C68">
+        <v>1363203.589777557</v>
+      </c>
+      <c r="D68">
+        <v>2.99999998</v>
+      </c>
+      <c r="E68">
+        <v>20982985.68700553</v>
+      </c>
+      <c r="G68">
+        <v>321903714.794352</v>
+      </c>
+      <c r="H68">
+        <v>5</v>
+      </c>
+      <c r="I68">
+        <v>303764449.160993</v>
+      </c>
+      <c r="J68" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
base simulador atualizada (maio v2)
</commit_message>
<xml_diff>
--- a/Base Simulador.xlsx
+++ b/Base Simulador.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="11">
   <si>
     <t>KPI1</t>
   </si>
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -456,7 +456,7 @@
         <v>33686531.32457296</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>93328618.23009101</v>
@@ -488,7 +488,7 @@
         <v>-4332350.325584246</v>
       </c>
       <c r="F3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3">
         <v>103079563.372284</v>
@@ -529,7 +529,7 @@
         <v>5</v>
       </c>
       <c r="I4">
-        <v>53121362.2945006</v>
+        <v>53121362.2945007</v>
       </c>
       <c r="J4" t="s">
         <v>9</v>
@@ -549,7 +549,7 @@
         <v>5.999999985</v>
       </c>
       <c r="E5">
-        <v>13833365.16757777</v>
+        <v>13833365.16757776</v>
       </c>
       <c r="F5">
         <v>12</v>
@@ -651,7 +651,7 @@
         <v>5</v>
       </c>
       <c r="I8">
-        <v>49886784.6835634</v>
+        <v>49886784.6835633</v>
       </c>
       <c r="J8" t="s">
         <v>9</v>
@@ -674,7 +674,7 @@
         <v>4720467.70784786</v>
       </c>
       <c r="F9">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>89465155.19588719</v>
@@ -703,10 +703,10 @@
         <v>1.999999997</v>
       </c>
       <c r="E10">
-        <v>9447875.952797854</v>
+        <v>9447875.952797845</v>
       </c>
       <c r="F10">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <v>66879630.3622337</v>
@@ -790,19 +790,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>110810.418692</v>
+        <v>103907.158792</v>
       </c>
       <c r="C13">
         <v>304635.8107719819</v>
       </c>
       <c r="D13">
-        <v>1.999999985</v>
+        <v>0.999999986</v>
       </c>
       <c r="E13">
-        <v>14425098.89858874</v>
+        <v>9546561.498471471</v>
       </c>
       <c r="F13">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G13">
         <v>95636875.7250993</v>
@@ -811,7 +811,7 @@
         <v>5</v>
       </c>
       <c r="I13">
-        <v>86620609.10685951</v>
+        <v>78416605.398717</v>
       </c>
       <c r="J13" t="s">
         <v>9</v>
@@ -831,7 +831,7 @@
         <v>2.99999999</v>
       </c>
       <c r="E14">
-        <v>163899.529774836</v>
+        <v>163899.5297748353</v>
       </c>
       <c r="F14">
         <v>25</v>
@@ -866,7 +866,7 @@
         <v>3416998.1415625</v>
       </c>
       <c r="F15">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G15">
         <v>44799383.9370562</v>
@@ -898,7 +898,7 @@
         <v>-688448.9842057356</v>
       </c>
       <c r="F16">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G16">
         <v>57183396.5740578</v>
@@ -930,7 +930,7 @@
         <v>8032350.7650893</v>
       </c>
       <c r="F17">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17">
         <v>140443579.463008</v>
@@ -994,7 +994,7 @@
         <v>9630383.649145005</v>
       </c>
       <c r="F19">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G19">
         <v>57316305.532588</v>
@@ -1026,7 +1026,7 @@
         <v>12709479.21787969</v>
       </c>
       <c r="F20">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G20">
         <v>32909016.7893645</v>
@@ -1067,7 +1067,7 @@
         <v>5</v>
       </c>
       <c r="I21">
-        <v>50942225.2829145</v>
+        <v>50942225.2829144</v>
       </c>
       <c r="J21" t="s">
         <v>9</v>
@@ -1087,10 +1087,10 @@
         <v>0.9999999939999999</v>
       </c>
       <c r="E22">
-        <v>8735829.482966226</v>
+        <v>8735829.482966224</v>
       </c>
       <c r="F22">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G22">
         <v>69444871.20746569</v>
@@ -1247,7 +1247,7 @@
         <v>3.999999989</v>
       </c>
       <c r="E27">
-        <v>-5273485.495753588</v>
+        <v>-5273485.49575359</v>
       </c>
       <c r="F27">
         <v>20</v>
@@ -1259,7 +1259,7 @@
         <v>5</v>
       </c>
       <c r="I27">
-        <v>75236861.7829894</v>
+        <v>75236861.78298929</v>
       </c>
       <c r="J27" t="s">
         <v>9</v>
@@ -1381,7 +1381,7 @@
         <v>5</v>
       </c>
       <c r="I31">
-        <v>54015049.9983958</v>
+        <v>54015049.9983959</v>
       </c>
       <c r="J31" t="s">
         <v>9</v>
@@ -1404,7 +1404,7 @@
         <v>49143446.77005175</v>
       </c>
       <c r="F32">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G32">
         <v>40319445.5433506</v>
@@ -1464,6 +1464,9 @@
       <c r="E34">
         <v>14129465.69103084</v>
       </c>
+      <c r="F34">
+        <v>22</v>
+      </c>
       <c r="H34">
         <v>5</v>
       </c>
@@ -1488,7 +1491,10 @@
         <v>-9E-09</v>
       </c>
       <c r="E35">
-        <v>-7245394.153791307</v>
+        <v>-7245394.153791296</v>
+      </c>
+      <c r="F35">
+        <v>17</v>
       </c>
       <c r="G35">
         <v>462914368.036666</v>
@@ -1519,6 +1525,9 @@
       <c r="E36">
         <v>15674217.66116987</v>
       </c>
+      <c r="F36">
+        <v>30</v>
+      </c>
       <c r="G36">
         <v>162971737.218567</v>
       </c>
@@ -1526,7 +1535,7 @@
         <v>5</v>
       </c>
       <c r="I36">
-        <v>140937442.588492</v>
+        <v>140937442.588491</v>
       </c>
       <c r="J36" t="s">
         <v>10</v>
@@ -1546,7 +1555,10 @@
         <v>1.99999999</v>
       </c>
       <c r="E37">
-        <v>19674320.38476177</v>
+        <v>19674320.38476176</v>
+      </c>
+      <c r="F37">
+        <v>13</v>
       </c>
       <c r="G37">
         <v>165949842.129764</v>
@@ -1575,7 +1587,10 @@
         <v>7.999999976</v>
       </c>
       <c r="E38">
-        <v>27574170.14620421</v>
+        <v>27574170.14620422</v>
+      </c>
+      <c r="F38">
+        <v>5</v>
       </c>
       <c r="G38">
         <v>195397061.094805</v>
@@ -1601,7 +1616,10 @@
         <v>-2E-08</v>
       </c>
       <c r="E39">
-        <v>9073580.796574228</v>
+        <v>9073580.796574241</v>
+      </c>
+      <c r="F39">
+        <v>16</v>
       </c>
       <c r="H39">
         <v>5</v>
@@ -1627,7 +1645,10 @@
         <v>0.9999999939999999</v>
       </c>
       <c r="E40">
-        <v>2744269.595138839</v>
+        <v>2744269.59513884</v>
+      </c>
+      <c r="F40">
+        <v>27</v>
       </c>
       <c r="G40">
         <v>264508335.976307</v>
@@ -1656,7 +1677,10 @@
         <v>-4.000000007</v>
       </c>
       <c r="E41">
-        <v>22689221.6004031</v>
+        <v>22765456.63839758</v>
+      </c>
+      <c r="F41">
+        <v>32</v>
       </c>
       <c r="G41">
         <v>180773023.234012</v>
@@ -1684,6 +1708,9 @@
       <c r="E42">
         <v>21084562.53407755</v>
       </c>
+      <c r="F42">
+        <v>6</v>
+      </c>
       <c r="H42">
         <v>5</v>
       </c>
@@ -1708,7 +1735,10 @@
         <v>-2.000000014</v>
       </c>
       <c r="E43">
-        <v>8365578.784704198</v>
+        <v>8365578.784704199</v>
+      </c>
+      <c r="F43">
+        <v>31</v>
       </c>
       <c r="G43">
         <v>269938285.450157</v>
@@ -1739,6 +1769,9 @@
       <c r="E44">
         <v>67699177.56819198</v>
       </c>
+      <c r="F44">
+        <v>8</v>
+      </c>
       <c r="G44">
         <v>453930494.313569</v>
       </c>
@@ -1766,10 +1799,13 @@
         <v>-1.000000039</v>
       </c>
       <c r="E45">
-        <v>30991267.53152352</v>
+        <v>31097026.64363621</v>
+      </c>
+      <c r="F45">
+        <v>7</v>
       </c>
       <c r="G45">
-        <v>349123366.348481</v>
+        <v>338347044.616148</v>
       </c>
       <c r="H45">
         <v>5</v>
@@ -1795,7 +1831,10 @@
         <v>4.999999985</v>
       </c>
       <c r="E46">
-        <v>37792529.97965544</v>
+        <v>37792529.97965543</v>
+      </c>
+      <c r="F46">
+        <v>24</v>
       </c>
       <c r="G46">
         <v>871844868.1560791</v>
@@ -1826,6 +1865,9 @@
       <c r="E47">
         <v>1489812.729699546</v>
       </c>
+      <c r="F47">
+        <v>28</v>
+      </c>
       <c r="G47">
         <v>392707751.013488</v>
       </c>
@@ -1855,6 +1897,9 @@
       <c r="E48">
         <v>4327483.929702809</v>
       </c>
+      <c r="F48">
+        <v>25</v>
+      </c>
       <c r="G48">
         <v>127932972.017863</v>
       </c>
@@ -1873,7 +1918,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>330437.0770120001</v>
+        <v>330437.077012</v>
       </c>
       <c r="C49">
         <v>782269.404911224</v>
@@ -1883,6 +1928,9 @@
       </c>
       <c r="E49">
         <v>9157319.962886602</v>
+      </c>
+      <c r="F49">
+        <v>29</v>
       </c>
       <c r="G49">
         <v>188896780.837437</v>
@@ -1908,7 +1956,10 @@
         <v>11.999999967</v>
       </c>
       <c r="E50">
-        <v>99004889.16466613</v>
+        <v>99004889.16466612</v>
+      </c>
+      <c r="F50">
+        <v>10</v>
       </c>
       <c r="H50">
         <v>5</v>
@@ -1936,6 +1987,9 @@
       <c r="E51">
         <v>-4070848.855628334</v>
       </c>
+      <c r="F51">
+        <v>26</v>
+      </c>
       <c r="G51">
         <v>353258554.43773</v>
       </c>
@@ -1954,25 +2008,28 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>1316923.272999999</v>
+        <v>399500.4786539997</v>
       </c>
       <c r="C52">
-        <v>1209583.366300517</v>
+        <v>1479373.320258577</v>
       </c>
       <c r="D52">
-        <v>0.999999984</v>
+        <v>0.999999985</v>
       </c>
       <c r="E52">
-        <v>20948099.12176</v>
+        <v>2406525.90925815</v>
+      </c>
+      <c r="F52">
+        <v>33</v>
       </c>
       <c r="G52">
-        <v>393097049.230891</v>
+        <v>349335762.370402</v>
       </c>
       <c r="H52">
         <v>5</v>
       </c>
       <c r="I52">
-        <v>399360239.004852</v>
+        <v>285022400.390091</v>
       </c>
       <c r="J52" t="s">
         <v>10</v>
@@ -1983,25 +2040,28 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>399500.4786539997</v>
+        <v>1664608.373266002</v>
       </c>
       <c r="C53">
-        <v>1479373.320258577</v>
+        <v>2343958.091319741</v>
       </c>
       <c r="D53">
-        <v>0.999999985</v>
+        <v>5.999999982</v>
       </c>
       <c r="E53">
-        <v>2406525.909258162</v>
+        <v>36880788.4355883</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
       </c>
       <c r="G53">
-        <v>349335762.370402</v>
+        <v>490132517.48139</v>
       </c>
       <c r="H53">
         <v>5</v>
       </c>
       <c r="I53">
-        <v>285022400.390091</v>
+        <v>475500342.421061</v>
       </c>
       <c r="J53" t="s">
         <v>10</v>
@@ -2012,25 +2072,22 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>1664608.373266002</v>
-      </c>
-      <c r="C54">
-        <v>2343958.091319741</v>
+        <v>1192790.478853999</v>
       </c>
       <c r="D54">
-        <v>5.999999982</v>
+        <v>-5.000000029</v>
       </c>
       <c r="E54">
-        <v>36880788.4355883</v>
-      </c>
-      <c r="G54">
-        <v>490132517.48139</v>
+        <v>24041690.26878395</v>
+      </c>
+      <c r="F54">
+        <v>21</v>
       </c>
       <c r="H54">
         <v>5</v>
       </c>
       <c r="I54">
-        <v>475500342.421061</v>
+        <v>499237175.937533</v>
       </c>
       <c r="J54" t="s">
         <v>10</v>
@@ -2041,19 +2098,28 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>1192790.478853999</v>
+        <v>295237.1833050001</v>
+      </c>
+      <c r="C55">
+        <v>766539.41086116</v>
       </c>
       <c r="D55">
-        <v>-5.000000029</v>
+        <v>0.999999991</v>
       </c>
       <c r="E55">
-        <v>24041690.26878395</v>
+        <v>-2412282.298719347</v>
+      </c>
+      <c r="F55">
+        <v>34</v>
+      </c>
+      <c r="G55">
+        <v>181008866.249681</v>
       </c>
       <c r="H55">
         <v>5</v>
       </c>
       <c r="I55">
-        <v>499237175.937533</v>
+        <v>150776833.048063</v>
       </c>
       <c r="J55" t="s">
         <v>10</v>
@@ -2064,25 +2130,28 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>295237.1833050001</v>
+        <v>559147.208685</v>
       </c>
       <c r="C56">
-        <v>766539.41086116</v>
+        <v>671990.759055843</v>
       </c>
       <c r="D56">
-        <v>0.999999991</v>
+        <v>4.999999989</v>
       </c>
       <c r="E56">
-        <v>-2412282.298719347</v>
+        <v>46342348.84790082</v>
+      </c>
+      <c r="F56">
+        <v>9</v>
       </c>
       <c r="G56">
-        <v>181008866.249681</v>
+        <v>280524877.955404</v>
       </c>
       <c r="H56">
         <v>5</v>
       </c>
       <c r="I56">
-        <v>150776833.048063</v>
+        <v>238815037.368466</v>
       </c>
       <c r="J56" t="s">
         <v>10</v>
@@ -2093,25 +2162,28 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>559147.208685</v>
+        <v>948751.756936</v>
       </c>
       <c r="C57">
-        <v>671990.759055843</v>
+        <v>1075185.214489349</v>
       </c>
       <c r="D57">
-        <v>4.999999989</v>
+        <v>2.999999982</v>
       </c>
       <c r="E57">
-        <v>46342348.84790082</v>
+        <v>19574394.36861564</v>
+      </c>
+      <c r="F57">
+        <v>4</v>
       </c>
       <c r="G57">
-        <v>280524877.955404</v>
+        <v>443866203.113601</v>
       </c>
       <c r="H57">
         <v>5</v>
       </c>
       <c r="I57">
-        <v>238815037.368466</v>
+        <v>402289284.770168</v>
       </c>
       <c r="J57" t="s">
         <v>10</v>
@@ -2122,25 +2194,28 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>948751.756936</v>
+        <v>1030383.516133</v>
       </c>
       <c r="C58">
         <v>1075185.214489349</v>
       </c>
       <c r="D58">
-        <v>2.999999982</v>
+        <v>2.999999985</v>
       </c>
       <c r="E58">
-        <v>19574394.36861564</v>
+        <v>-18291582.73189784</v>
+      </c>
+      <c r="F58">
+        <v>11</v>
       </c>
       <c r="G58">
-        <v>443866203.113601</v>
+        <v>435872490.965229</v>
       </c>
       <c r="H58">
         <v>5</v>
       </c>
       <c r="I58">
-        <v>402289284.770169</v>
+        <v>372284378.690909</v>
       </c>
       <c r="J58" t="s">
         <v>10</v>
@@ -2151,25 +2226,28 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>1030383.516133</v>
+        <v>867290.346103</v>
       </c>
       <c r="C59">
         <v>1075185.214489349</v>
       </c>
       <c r="D59">
-        <v>2.999999985</v>
+        <v>-1.1E-08</v>
       </c>
       <c r="E59">
-        <v>-18291582.73189784</v>
+        <v>-16038339.70004725</v>
+      </c>
+      <c r="F59">
+        <v>20</v>
       </c>
       <c r="G59">
-        <v>435872490.965229</v>
+        <v>534243142.793327</v>
       </c>
       <c r="H59">
         <v>5</v>
       </c>
       <c r="I59">
-        <v>372284378.690909</v>
+        <v>464730008.847567</v>
       </c>
       <c r="J59" t="s">
         <v>10</v>
@@ -2180,25 +2258,28 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>867290.346103</v>
+        <v>830777.7814730001</v>
       </c>
       <c r="C60">
         <v>1075185.214489349</v>
       </c>
       <c r="D60">
-        <v>-1.1E-08</v>
+        <v>-1.2E-08</v>
       </c>
       <c r="E60">
-        <v>-16088246.30951444</v>
+        <v>-7755943.792864057</v>
+      </c>
+      <c r="F60">
+        <v>15</v>
       </c>
       <c r="G60">
-        <v>523466821.060994</v>
+        <v>347512645.701532</v>
       </c>
       <c r="H60">
         <v>5</v>
       </c>
       <c r="I60">
-        <v>464730008.847567</v>
+        <v>403819992.292377</v>
       </c>
       <c r="J60" t="s">
         <v>10</v>
@@ -2209,25 +2290,28 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>830777.7814730001</v>
+        <v>847785.775594</v>
       </c>
       <c r="C61">
         <v>1075185.214489349</v>
       </c>
       <c r="D61">
-        <v>-1.2E-08</v>
+        <v>-2.000000013</v>
       </c>
       <c r="E61">
-        <v>-7755943.79286405</v>
+        <v>14885126.86672064</v>
+      </c>
+      <c r="F61">
+        <v>12</v>
       </c>
       <c r="G61">
-        <v>347512645.701532</v>
+        <v>405377230.617039</v>
       </c>
       <c r="H61">
         <v>5</v>
       </c>
       <c r="I61">
-        <v>403819992.292377</v>
+        <v>390448045.247282</v>
       </c>
       <c r="J61" t="s">
         <v>10</v>
@@ -2238,25 +2322,28 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>847785.775594</v>
+        <v>463968.8240989997</v>
       </c>
       <c r="C62">
-        <v>1075185.214489349</v>
+        <v>761589.526929955</v>
       </c>
       <c r="D62">
-        <v>-2.000000013</v>
+        <v>4.999999982</v>
       </c>
       <c r="E62">
-        <v>14885126.86672064</v>
+        <v>16970925.28966692</v>
+      </c>
+      <c r="F62">
+        <v>19</v>
       </c>
       <c r="G62">
-        <v>405377230.617039</v>
+        <v>310420875.883594</v>
       </c>
       <c r="H62">
         <v>5</v>
       </c>
       <c r="I62">
-        <v>390448045.247282</v>
+        <v>313137532.893437</v>
       </c>
       <c r="J62" t="s">
         <v>10</v>
@@ -2267,25 +2354,28 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>463968.8240989997</v>
+        <v>431734.2034979999</v>
       </c>
       <c r="C63">
-        <v>761589.526929955</v>
+        <v>456771.5319966288</v>
       </c>
       <c r="D63">
-        <v>4.999999982</v>
+        <v>1.999999992</v>
       </c>
       <c r="E63">
-        <v>16970925.28966693</v>
+        <v>5398299.655918254</v>
+      </c>
+      <c r="F63">
+        <v>18</v>
       </c>
       <c r="G63">
-        <v>310420875.883594</v>
+        <v>143247730.662296</v>
       </c>
       <c r="H63">
         <v>5</v>
       </c>
       <c r="I63">
-        <v>313137532.893437</v>
+        <v>127360244.329447</v>
       </c>
       <c r="J63" t="s">
         <v>10</v>
@@ -2296,25 +2386,22 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>431734.2034979999</v>
-      </c>
-      <c r="C64">
-        <v>456771.5319966288</v>
+        <v>3632141.897297002</v>
       </c>
       <c r="D64">
-        <v>1.999999992</v>
+        <v>4.999999965</v>
       </c>
       <c r="E64">
-        <v>5398299.655918254</v>
-      </c>
-      <c r="G64">
-        <v>143247730.662296</v>
+        <v>171051883.5710644</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
       </c>
       <c r="H64">
         <v>5</v>
       </c>
       <c r="I64">
-        <v>127360244.329447</v>
+        <v>1059393350.79388</v>
       </c>
       <c r="J64" t="s">
         <v>10</v>
@@ -2325,19 +2412,22 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>3632141.897297002</v>
+        <v>1404228.462323</v>
       </c>
       <c r="D65">
-        <v>4.999999965</v>
+        <v>0.999999976</v>
       </c>
       <c r="E65">
-        <v>171051883.5710644</v>
+        <v>16745936.93818602</v>
+      </c>
+      <c r="F65">
+        <v>14</v>
       </c>
       <c r="H65">
         <v>5</v>
       </c>
       <c r="I65">
-        <v>1059393350.79388</v>
+        <v>513017299.883275</v>
       </c>
       <c r="J65" t="s">
         <v>10</v>
@@ -2348,19 +2438,28 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>1410706.602323</v>
+        <v>708795.817177</v>
+      </c>
+      <c r="C66">
+        <v>940787.0626781799</v>
       </c>
       <c r="D66">
-        <v>-2.3E-08</v>
+        <v>-1.1E-08</v>
       </c>
       <c r="E66">
-        <v>15754357.8058238</v>
+        <v>-4735994.28343372</v>
+      </c>
+      <c r="F66">
+        <v>23</v>
+      </c>
+      <c r="G66">
+        <v>642220644.6680959</v>
       </c>
       <c r="H66">
         <v>5</v>
       </c>
       <c r="I66">
-        <v>512437199.742186</v>
+        <v>602016352.158518</v>
       </c>
       <c r="J66" t="s">
         <v>10</v>
@@ -2371,56 +2470,30 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>708795.817177</v>
+        <v>1117577.921944003</v>
       </c>
       <c r="C67">
-        <v>940787.0626781799</v>
+        <v>1363203.589777557</v>
       </c>
       <c r="D67">
-        <v>-1.1E-08</v>
+        <v>2.99999998</v>
       </c>
       <c r="E67">
-        <v>-4735994.28343373</v>
+        <v>20982985.68700553</v>
+      </c>
+      <c r="F67">
+        <v>3</v>
       </c>
       <c r="G67">
-        <v>642220644.6680959</v>
+        <v>321903714.794352</v>
       </c>
       <c r="H67">
         <v>5</v>
       </c>
       <c r="I67">
-        <v>602016352.158518</v>
+        <v>303764449.160994</v>
       </c>
       <c r="J67" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
-      <c r="A68" s="1">
-        <v>66</v>
-      </c>
-      <c r="B68">
-        <v>1117577.921944003</v>
-      </c>
-      <c r="C68">
-        <v>1363203.589777557</v>
-      </c>
-      <c r="D68">
-        <v>2.99999998</v>
-      </c>
-      <c r="E68">
-        <v>20982985.68700553</v>
-      </c>
-      <c r="G68">
-        <v>321903714.794352</v>
-      </c>
-      <c r="H68">
-        <v>5</v>
-      </c>
-      <c r="I68">
-        <v>303764449.160993</v>
-      </c>
-      <c r="J68" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
novo update da base do simulador
</commit_message>
<xml_diff>
--- a/Base Simulador.xlsx
+++ b/Base Simulador.xlsx
@@ -453,7 +453,7 @@
         <v>0.999999995</v>
       </c>
       <c r="E2">
-        <v>33686531.32457296</v>
+        <v>33686531.32457295</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -517,7 +517,7 @@
         <v>-7E-09</v>
       </c>
       <c r="E4">
-        <v>6872304.585514694</v>
+        <v>6872304.585514704</v>
       </c>
       <c r="F4">
         <v>19</v>
@@ -606,6 +606,9 @@
       <c r="B7">
         <v>279246.515913</v>
       </c>
+      <c r="C7">
+        <v>525595.3322263303</v>
+      </c>
       <c r="D7">
         <v>4.999999985</v>
       </c>
@@ -614,6 +617,9 @@
       </c>
       <c r="F7">
         <v>2</v>
+      </c>
+      <c r="G7">
+        <v>117220857.186105</v>
       </c>
       <c r="H7">
         <v>5</v>
@@ -651,7 +657,7 @@
         <v>5</v>
       </c>
       <c r="I8">
-        <v>49886784.6835633</v>
+        <v>49886784.6835634</v>
       </c>
       <c r="J8" t="s">
         <v>9</v>
@@ -703,7 +709,7 @@
         <v>1.999999997</v>
       </c>
       <c r="E10">
-        <v>9447875.952797845</v>
+        <v>9447875.952797854</v>
       </c>
       <c r="F10">
         <v>28</v>
@@ -831,7 +837,7 @@
         <v>2.99999999</v>
       </c>
       <c r="E14">
-        <v>163899.5297748353</v>
+        <v>163899.5297748352</v>
       </c>
       <c r="F14">
         <v>25</v>
@@ -927,7 +933,7 @@
         <v>0.999999993</v>
       </c>
       <c r="E17">
-        <v>8032350.7650893</v>
+        <v>8032350.765089288</v>
       </c>
       <c r="F17">
         <v>22</v>
@@ -1247,7 +1253,7 @@
         <v>3.999999989</v>
       </c>
       <c r="E27">
-        <v>-5273485.49575359</v>
+        <v>-5273485.495753591</v>
       </c>
       <c r="F27">
         <v>20</v>
@@ -1311,7 +1317,7 @@
         <v>0.999999995</v>
       </c>
       <c r="E29">
-        <v>9585279.296527943</v>
+        <v>9585279.296527933</v>
       </c>
       <c r="F29">
         <v>18</v>
@@ -1368,6 +1374,9 @@
       <c r="B31">
         <v>113004.929588</v>
       </c>
+      <c r="C31">
+        <v>258318.683726668</v>
+      </c>
       <c r="D31">
         <v>10.999999979</v>
       </c>
@@ -1377,11 +1386,14 @@
       <c r="F31">
         <v>7</v>
       </c>
+      <c r="G31">
+        <v>50438406.8982071</v>
+      </c>
       <c r="H31">
         <v>5</v>
       </c>
       <c r="I31">
-        <v>54015049.9983959</v>
+        <v>54015049.9983958</v>
       </c>
       <c r="J31" t="s">
         <v>9</v>
@@ -1433,7 +1445,7 @@
         <v>2.999999992</v>
       </c>
       <c r="E33">
-        <v>6069764.464888243</v>
+        <v>6069764.464888245</v>
       </c>
       <c r="F33">
         <v>14</v>
@@ -1458,6 +1470,9 @@
       <c r="B34">
         <v>437041.5331989997</v>
       </c>
+      <c r="C34">
+        <v>585527.948057324</v>
+      </c>
       <c r="D34">
         <v>4.999999985</v>
       </c>
@@ -1466,6 +1481,9 @@
       </c>
       <c r="F34">
         <v>22</v>
+      </c>
+      <c r="G34">
+        <v>240162116.010487</v>
       </c>
       <c r="H34">
         <v>5</v>
@@ -1491,7 +1509,7 @@
         <v>-9E-09</v>
       </c>
       <c r="E35">
-        <v>-7245394.153791296</v>
+        <v>-7245394.153791295</v>
       </c>
       <c r="F35">
         <v>17</v>
@@ -1523,7 +1541,7 @@
         <v>4.999999993</v>
       </c>
       <c r="E36">
-        <v>15674217.66116987</v>
+        <v>15674217.66116988</v>
       </c>
       <c r="F36">
         <v>30</v>
@@ -1535,7 +1553,7 @@
         <v>5</v>
       </c>
       <c r="I36">
-        <v>140937442.588491</v>
+        <v>140937442.588492</v>
       </c>
       <c r="J36" t="s">
         <v>10</v>
@@ -1555,7 +1573,7 @@
         <v>1.99999999</v>
       </c>
       <c r="E37">
-        <v>19674320.38476176</v>
+        <v>19674320.38476177</v>
       </c>
       <c r="F37">
         <v>13</v>
@@ -1587,7 +1605,7 @@
         <v>7.999999976</v>
       </c>
       <c r="E38">
-        <v>27574170.14620422</v>
+        <v>27574170.14620421</v>
       </c>
       <c r="F38">
         <v>5</v>
@@ -1612,14 +1630,20 @@
       <c r="B39">
         <v>1166441.761158001</v>
       </c>
+      <c r="C39">
+        <v>1986971.395975875</v>
+      </c>
       <c r="D39">
         <v>-2E-08</v>
       </c>
       <c r="E39">
-        <v>9073580.796574241</v>
+        <v>9073580.796574228</v>
       </c>
       <c r="F39">
         <v>16</v>
+      </c>
+      <c r="G39">
+        <v>359549616.289326</v>
       </c>
       <c r="H39">
         <v>5</v>
@@ -1645,7 +1669,7 @@
         <v>0.9999999939999999</v>
       </c>
       <c r="E40">
-        <v>2744269.59513884</v>
+        <v>2744269.595138839</v>
       </c>
       <c r="F40">
         <v>27</v>
@@ -1702,6 +1726,9 @@
       <c r="B42">
         <v>485061.0454419998</v>
       </c>
+      <c r="C42">
+        <v>560592.6138586564</v>
+      </c>
       <c r="D42">
         <v>1.999999985</v>
       </c>
@@ -1710,6 +1737,9 @@
       </c>
       <c r="F42">
         <v>6</v>
+      </c>
+      <c r="G42">
+        <v>138921011.0633</v>
       </c>
       <c r="H42">
         <v>5</v>
@@ -1735,7 +1765,7 @@
         <v>-2.000000014</v>
       </c>
       <c r="E43">
-        <v>8365578.784704199</v>
+        <v>8365578.784704204</v>
       </c>
       <c r="F43">
         <v>31</v>
@@ -1767,7 +1797,7 @@
         <v>8.999999957</v>
       </c>
       <c r="E44">
-        <v>67699177.56819198</v>
+        <v>67699177.56819201</v>
       </c>
       <c r="F44">
         <v>8</v>
@@ -1799,7 +1829,7 @@
         <v>-1.000000039</v>
       </c>
       <c r="E45">
-        <v>31097026.64363621</v>
+        <v>31097026.64363619</v>
       </c>
       <c r="F45">
         <v>7</v>
@@ -1831,7 +1861,7 @@
         <v>4.999999985</v>
       </c>
       <c r="E46">
-        <v>37792529.97965543</v>
+        <v>37792529.97965544</v>
       </c>
       <c r="F46">
         <v>24</v>
@@ -1863,7 +1893,7 @@
         <v>-1.000000008</v>
       </c>
       <c r="E47">
-        <v>1489812.729699546</v>
+        <v>1489812.729699545</v>
       </c>
       <c r="F47">
         <v>28</v>
@@ -1952,14 +1982,20 @@
       <c r="B50">
         <v>704143.3872839999</v>
       </c>
+      <c r="C50">
+        <v>1318373.742259424</v>
+      </c>
       <c r="D50">
         <v>11.999999967</v>
       </c>
       <c r="E50">
-        <v>99004889.16466612</v>
+        <v>99142898.92025533</v>
       </c>
       <c r="F50">
         <v>10</v>
+      </c>
+      <c r="G50">
+        <v>311861775.963436</v>
       </c>
       <c r="H50">
         <v>5</v>
@@ -2017,7 +2053,7 @@
         <v>0.999999985</v>
       </c>
       <c r="E52">
-        <v>2406525.90925815</v>
+        <v>2406525.909258161</v>
       </c>
       <c r="F52">
         <v>33</v>
@@ -2074,14 +2110,20 @@
       <c r="B54">
         <v>1192790.478853999</v>
       </c>
+      <c r="C54">
+        <v>2557827.666945276</v>
+      </c>
       <c r="D54">
         <v>-5.000000029</v>
       </c>
       <c r="E54">
-        <v>24041690.26878395</v>
+        <v>24041690.26878396</v>
       </c>
       <c r="F54">
         <v>21</v>
+      </c>
+      <c r="G54">
+        <v>552717606.141346</v>
       </c>
       <c r="H54">
         <v>5</v>
@@ -2139,7 +2181,7 @@
         <v>4.999999989</v>
       </c>
       <c r="E56">
-        <v>46342348.84790082</v>
+        <v>46342348.84790083</v>
       </c>
       <c r="F56">
         <v>9</v>
@@ -2235,7 +2277,7 @@
         <v>-1.1E-08</v>
       </c>
       <c r="E59">
-        <v>-16038339.70004725</v>
+        <v>-16038339.70004726</v>
       </c>
       <c r="F59">
         <v>20</v>
@@ -2267,7 +2309,7 @@
         <v>-1.2E-08</v>
       </c>
       <c r="E60">
-        <v>-7755943.792864057</v>
+        <v>-7739752.17270211</v>
       </c>
       <c r="F60">
         <v>15</v>
@@ -2354,7 +2396,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>431734.2034979999</v>
+        <v>431734.2034979998</v>
       </c>
       <c r="C63">
         <v>456771.5319966288</v>
@@ -2363,7 +2405,7 @@
         <v>1.999999992</v>
       </c>
       <c r="E63">
-        <v>5398299.655918254</v>
+        <v>5398299.655918255</v>
       </c>
       <c r="F63">
         <v>18</v>
@@ -2388,6 +2430,9 @@
       <c r="B64">
         <v>3632141.897297002</v>
       </c>
+      <c r="C64">
+        <v>4730814.943753129</v>
+      </c>
       <c r="D64">
         <v>4.999999965</v>
       </c>
@@ -2396,6 +2441,9 @@
       </c>
       <c r="F64">
         <v>1</v>
+      </c>
+      <c r="G64">
+        <v>1006967360.25823</v>
       </c>
       <c r="H64">
         <v>5</v>
@@ -2414,14 +2462,20 @@
       <c r="B65">
         <v>1404228.462323</v>
       </c>
+      <c r="C65">
+        <v>2436212.450195243</v>
+      </c>
       <c r="D65">
         <v>0.999999976</v>
       </c>
       <c r="E65">
-        <v>16745936.93818602</v>
+        <v>16745936.93818601</v>
       </c>
       <c r="F65">
         <v>14</v>
+      </c>
+      <c r="G65">
+        <v>571824545.031608</v>
       </c>
       <c r="H65">
         <v>5</v>
@@ -2447,7 +2501,7 @@
         <v>-1.1E-08</v>
       </c>
       <c r="E66">
-        <v>-4735994.28343372</v>
+        <v>-4735994.283433722</v>
       </c>
       <c r="F66">
         <v>23</v>
@@ -2479,7 +2533,7 @@
         <v>2.99999998</v>
       </c>
       <c r="E67">
-        <v>20982985.68700553</v>
+        <v>20982985.68700554</v>
       </c>
       <c r="F67">
         <v>3</v>
@@ -2491,7 +2545,7 @@
         <v>5</v>
       </c>
       <c r="I67">
-        <v>303764449.160994</v>
+        <v>303764449.160993</v>
       </c>
       <c r="J67" t="s">
         <v>10</v>

</xml_diff>